<commit_message>
Add data processing and visualization script for shot data analysis
</commit_message>
<xml_diff>
--- a/Shot_Data/AI_caddie_shot_data_test.xlsx
+++ b/Shot_Data/AI_caddie_shot_data_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacksonne/Python Projects/AI_Caddie/Shot_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89BD5F91-DB20-FE49-A9CC-F17B1493D573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB007180-E8D9-254B-BE5A-7C6496AC83D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6780" yWindow="5960" windowWidth="14460" windowHeight="9940" xr2:uid="{1DBDA87C-0B9C-A74B-8865-649EAEC11D66}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>Player</t>
   </si>
@@ -113,6 +113,24 @@
   </si>
   <si>
     <t>Not full, but not knockdown</t>
+  </si>
+  <si>
+    <t>Brock Rumpke</t>
+  </si>
+  <si>
+    <t>5 iron</t>
+  </si>
+  <si>
+    <t>Srixon ZX5</t>
+  </si>
+  <si>
+    <t>Dynamic Gold X100</t>
+  </si>
+  <si>
+    <t>Full Fade</t>
+  </si>
+  <si>
+    <t>Normal shot, hitting a fade</t>
   </si>
 </sst>
 </file>
@@ -148,8 +166,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -172,8 +191,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C4C1572-458A-6A4B-B5CF-4FDE539DD7A3}" name="Table1" displayName="Table1" ref="A1:S6" totalsRowShown="0">
-  <autoFilter ref="A1:S6" xr:uid="{4C4C1572-458A-6A4B-B5CF-4FDE539DD7A3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C4C1572-458A-6A4B-B5CF-4FDE539DD7A3}" name="Table1" displayName="Table1" ref="A1:S7" totalsRowShown="0">
+  <autoFilter ref="A1:S7" xr:uid="{4C4C1572-458A-6A4B-B5CF-4FDE539DD7A3}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{E7293B6A-8EA5-E94A-98F2-7602667D5089}" name="Player"/>
     <tableColumn id="18" xr3:uid="{BDBDB812-3599-3D46-A682-AB5A9B2A1401}" name="Club"/>
@@ -498,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7E9260-9C54-5E48-97BF-FEFB4A2B8F76}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -888,6 +907,66 @@
         <v>25</v>
       </c>
     </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>208</v>
+      </c>
+      <c r="D7">
+        <v>207.1</v>
+      </c>
+      <c r="E7">
+        <v>220</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7">
+        <v>136</v>
+      </c>
+      <c r="J7">
+        <v>13</v>
+      </c>
+      <c r="K7">
+        <v>4000</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>95</v>
+      </c>
+      <c r="N7" s="1">
+        <f>Table1[[#This Row],[Ball Speed (mph)]]/Table1[[#This Row],[Club Speed (mph)]]</f>
+        <v>1.4315789473684211</v>
+      </c>
+      <c r="O7">
+        <v>-2</v>
+      </c>
+      <c r="P7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" t="s">
+        <v>30</v>
+      </c>
+      <c r="S7" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>